<commit_message>
all ready to receive database from characters, fotos and biscoitos
</commit_message>
<xml_diff>
--- a/script/data/ika-database.xlsx
+++ b/script/data/ika-database.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="characters" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="fotos" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="biscoito" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="538">
   <si>
     <t>nick</t>
   </si>
@@ -344,6 +345,12 @@
     <t>https://img2.finalfantasyxiv.com/f/987051a015b046845a40ff1d5e446e9d_be20385e18333edb329d4574f364a1f0fc0_96x96.jpg?1657036712</t>
   </si>
   <si>
+    <t>Chloe Facca</t>
+  </si>
+  <si>
+    <t>https://img2.finalfantasyxiv.com/f/f095e0eecc1b77173f4d31187e1b8e18_be20385e18333edb329d4574f364a1f0fc0_96x96.jpg?1657042496</t>
+  </si>
+  <si>
     <t>fileName</t>
   </si>
   <si>
@@ -1482,13 +1489,151 @@
   </si>
   <si>
     <t>img/screenshots/fotos/2020/social/tengu-stack.png</t>
+  </si>
+  <si>
+    <t>expansion</t>
+  </si>
+  <si>
+    <t>dutyName</t>
+  </si>
+  <si>
+    <t>dutyLevel</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p1job</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p2job</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>p3job</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>p4job</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>p5job</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>p6job</t>
+  </si>
+  <si>
+    <t>p7</t>
+  </si>
+  <si>
+    <t>p7job</t>
+  </si>
+  <si>
+    <t>p8</t>
+  </si>
+  <si>
+    <t>p8job</t>
+  </si>
+  <si>
+    <t>e5s_kenji</t>
+  </si>
+  <si>
+    <t>shb</t>
+  </si>
+  <si>
+    <t>Eden's Verse: Fulmination</t>
+  </si>
+  <si>
+    <t>savage</t>
+  </si>
+  <si>
+    <t>img/screenshots/biscoito/2020/e5s-kenji.png</t>
+  </si>
+  <si>
+    <t>pld</t>
+  </si>
+  <si>
+    <t>chloefacca</t>
+  </si>
+  <si>
+    <t>war</t>
+  </si>
+  <si>
+    <t>yesodketer</t>
+  </si>
+  <si>
+    <t>whm</t>
+  </si>
+  <si>
+    <t>ast</t>
+  </si>
+  <si>
+    <t>sam</t>
+  </si>
+  <si>
+    <t>drg</t>
+  </si>
+  <si>
+    <t>rirururiru</t>
+  </si>
+  <si>
+    <t>brd</t>
+  </si>
+  <si>
+    <t>ygglart</t>
+  </si>
+  <si>
+    <t>rdm</t>
+  </si>
+  <si>
+    <t>t9_kenji</t>
+  </si>
+  <si>
+    <t>arr</t>
+  </si>
+  <si>
+    <t>16/06/2020</t>
+  </si>
+  <si>
+    <t>Second Coil of Bahamut, Turn 4</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>img/screenshots/biscoito/2020/t9-kenji.png</t>
+  </si>
+  <si>
+    <t>lilinawada</t>
+  </si>
+  <si>
+    <t>nyardodix</t>
+  </si>
+  <si>
+    <t>kaliweiss</t>
+  </si>
+  <si>
+    <t>smn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1510,8 +1655,12 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1524,6 +1673,12 @@
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -1531,7 +1686,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1542,6 +1697,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1557,6 +1718,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2470,7 +2635,20 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="2">
+        <v>3.0344429E7</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="52" ht="15.75" customHeight="1"/>
     <row r="53" ht="15.75" customHeight="1"/>
     <row r="54" ht="15.75" customHeight="1"/>
@@ -3471,8 +3649,9 @@
     <hyperlink r:id="rId47" ref="B48"/>
     <hyperlink r:id="rId48" ref="B49"/>
     <hyperlink r:id="rId49" ref="B50"/>
+    <hyperlink r:id="rId50" ref="B51"/>
   </hyperlinks>
-  <drawing r:id="rId50"/>
+  <drawing r:id="rId51"/>
 </worksheet>
 </file>
 
@@ -3488,2681 +3667,2900 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2">
         <v>2020.0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C5" s="2">
         <v>2020.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C6" s="2">
         <v>2020.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C7" s="2">
         <v>2020.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C8" s="2">
         <v>2020.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C10" s="2">
         <v>2020.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C12" s="2">
         <v>2020.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C13" s="2">
         <v>2020.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C14" s="2">
         <v>2020.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C15" s="2">
         <v>2020.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C16" s="2">
         <v>2020.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C17" s="2">
         <v>2020.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C18" s="2">
         <v>2020.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C19" s="2">
         <v>2020.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C20" s="2">
         <v>2020.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C21" s="2">
         <v>2020.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C22" s="2">
         <v>2020.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C23" s="2">
         <v>2020.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C24" s="2">
         <v>2020.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C25" s="2">
         <v>2020.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C26" s="2">
         <v>2020.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="C27" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C28" s="2">
         <v>2020.0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C29" s="2">
         <v>2020.0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C30" s="2">
         <v>2020.0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C31" s="2">
         <v>2020.0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C32" s="2">
         <v>2020.0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C33" s="2">
         <v>2020.0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C34" s="2">
         <v>2020.0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C35" s="2">
         <v>2020.0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C36" s="2">
         <v>2020.0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C37" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C38" s="2">
         <v>2020.0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C39" s="2">
         <v>2020.0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C40" s="2">
         <v>2020.0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C41" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="E41" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C42" s="2">
         <v>2020.0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C43" s="2">
         <v>2020.0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C44" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>248</v>
-      </c>
       <c r="E44" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C45" s="2">
         <v>2020.0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C46" s="2">
         <v>2020.0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C47" s="2">
         <v>2020.0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C48" s="2">
         <v>2020.0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C49" s="2">
         <v>2020.0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C50" s="2">
         <v>2020.0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C51" s="2">
         <v>2020.0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C52" s="2">
         <v>2020.0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C53" s="2">
         <v>2020.0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C54" s="2">
         <v>2020.0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C55" s="2">
         <v>2020.0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C56" s="2">
         <v>2020.0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C57" s="2">
         <v>2020.0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C58" s="2">
         <v>2020.0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C59" s="2">
         <v>2020.0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C60" s="2">
         <v>2020.0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C61" s="2">
         <v>2020.0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C62" s="2">
         <v>2020.0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C63" s="2">
         <v>2020.0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C64" s="2">
         <v>2020.0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C65" s="2">
         <v>2020.0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C66" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C66" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="E66" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C67" s="2">
         <v>2020.0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C68" s="2">
         <v>2020.0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C69" s="2">
         <v>2020.0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C70" s="2">
         <v>2020.0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C71" s="2">
         <v>2020.0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C72" s="2">
         <v>2020.0</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C73" s="2">
         <v>2020.0</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C74" s="2">
         <v>2020.0</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C75" s="2">
         <v>2020.0</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C76" s="2">
         <v>2020.0</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C77" s="2">
         <v>2020.0</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C78" s="2">
         <v>2020.0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C79" s="2">
         <v>2020.0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C80" s="2">
         <v>2020.0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C81" s="2">
         <v>2020.0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C82" s="2">
         <v>2020.0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C83" s="2">
         <v>2020.0</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C84" s="2">
         <v>2020.0</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C85" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F85" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="C85" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C86" s="2">
         <v>2020.0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C87" s="2">
         <v>2020.0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C88" s="2">
         <v>2020.0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C89" s="2">
         <v>2020.0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C90" s="2">
         <v>2020.0</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C91" s="2">
         <v>2020.0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C92" s="2">
         <v>2020.0</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C93" s="2">
         <v>2020.0</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C94" s="2">
         <v>2020.0</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C95" s="2">
         <v>2020.0</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C96" s="2">
         <v>2020.0</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C97" s="2">
         <v>2020.0</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C98" s="2">
         <v>2020.0</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C99" s="2">
         <v>2020.0</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C100" s="2">
         <v>2020.0</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C101" s="2">
         <v>2020.0</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C102" s="2">
         <v>2020.0</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C103" s="2">
         <v>2020.0</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C104" s="2">
         <v>2020.0</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C105" s="2">
         <v>2020.0</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C106" s="2">
         <v>2020.0</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C107" s="2">
         <v>2020.0</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C108" s="2">
         <v>2020.0</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C109" s="2">
         <v>2020.0</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C110" s="2">
         <v>2020.0</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C111" s="2">
         <v>2020.0</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C112" s="2">
         <v>2020.0</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C113" s="2">
         <v>2020.0</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C114" s="2">
         <v>2020.0</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C115" s="2">
         <v>2020.0</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C116" s="2">
         <v>2020.0</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C117" s="2">
         <v>2020.0</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C118" s="2">
         <v>2020.0</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C119" s="2">
         <v>2020.0</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C120" s="2">
         <v>2020.0</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C121" s="2">
         <v>2020.0</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C122" s="2">
         <v>2020.0</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C123" s="2">
         <v>2020.0</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C124" s="2">
         <v>2020.0</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C125" s="2">
         <v>2020.0</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C126" s="2">
         <v>2020.0</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C127" s="2">
         <v>2020.0</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C128" s="2">
         <v>2020.0</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C129" s="2">
         <v>2020.0</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C130" s="2">
         <v>2020.0</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C131" s="2">
         <v>2020.0</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C132" s="2">
         <v>2020.0</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C133" s="2">
         <v>2020.0</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C134" s="2">
         <v>2020.0</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C135" s="2">
         <v>2020.0</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C136" s="2">
         <v>2020.0</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C137" s="2">
         <v>2020.0</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C138" s="2">
         <v>2020.0</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C139" s="2">
         <v>2020.0</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C140" s="2">
         <v>2020.0</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C141" s="2">
         <v>2020.0</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2020.0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>